<commit_message>
No devuelve nada al chile
Programa de fracciones no funciona la parte que convierte string a int c:
</commit_message>
<xml_diff>
--- a/Parcial 1/Libro1.xlsx
+++ b/Parcial 1/Libro1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Documents\CETI\8vo\Programación Avanzada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Documents\CETI\8vo\Programación Avanzada\Avanzada\Parcial 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -339,7 +339,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>